<commit_message>
aggiunto import ranking da file
aggiunto import ranking da file
</commit_message>
<xml_diff>
--- a/export/ExportSerieA2018.xlsx
+++ b/export/ExportSerieA2018.xlsx
@@ -28,196 +28,196 @@
     <t>ODS</t>
   </si>
   <si>
+    <t>Atletico Lupin</t>
+  </si>
+  <si>
+    <t>Santaklaus</t>
+  </si>
+  <si>
+    <t>Cave Canem F.C.</t>
+  </si>
+  <si>
+    <t>Squaraus</t>
+  </si>
+  <si>
+    <t>Miami Sharks</t>
+  </si>
+  <si>
+    <t>Antoncasta</t>
+  </si>
+  <si>
+    <t>Jukatan</t>
+  </si>
+  <si>
+    <t>Juk</t>
+  </si>
+  <si>
+    <t>Pit Stop F.C.</t>
+  </si>
+  <si>
+    <t>Pit Stop</t>
+  </si>
+  <si>
+    <t>B.B. King</t>
+  </si>
+  <si>
+    <t>Remida</t>
+  </si>
+  <si>
+    <t>Ragni Domestici</t>
+  </si>
+  <si>
+    <t>Woland</t>
+  </si>
+  <si>
+    <t>Machu Picchu</t>
+  </si>
+  <si>
+    <t>Caniggia</t>
+  </si>
+  <si>
+    <t>Footbears F.C.</t>
+  </si>
+  <si>
+    <t>Fatbear</t>
+  </si>
+  <si>
+    <t>Fantatalanta</t>
+  </si>
+  <si>
+    <t>Federico</t>
+  </si>
+  <si>
+    <t>Armata Brancaleone</t>
+  </si>
+  <si>
+    <t>Vervex</t>
+  </si>
+  <si>
+    <t>Annabella</t>
+  </si>
+  <si>
+    <t>Zag</t>
+  </si>
+  <si>
+    <t>Younes F.C.</t>
+  </si>
+  <si>
+    <t>Yeboah</t>
+  </si>
+  <si>
+    <t>Ciak</t>
+  </si>
+  <si>
+    <t>Danbell</t>
+  </si>
+  <si>
+    <t>Real Mafra</t>
+  </si>
+  <si>
+    <t>Stef</t>
+  </si>
+  <si>
+    <t>Phoenix S.R.C.L.</t>
+  </si>
+  <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>Swansea F.C.</t>
+  </si>
+  <si>
+    <t>Swansea</t>
+  </si>
+  <si>
+    <t>Jeeg Robot</t>
+  </si>
+  <si>
+    <t>Hiroshi</t>
+  </si>
+  <si>
+    <t>A.S. Paulina Maria</t>
+  </si>
+  <si>
+    <t>Fede235</t>
+  </si>
+  <si>
+    <t>F.C. Ezio Glerean</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Trimonese</t>
+  </si>
+  <si>
+    <t>Korlos</t>
+  </si>
+  <si>
+    <t>Real Ultima</t>
+  </si>
+  <si>
+    <t>Mark Mol</t>
+  </si>
+  <si>
+    <t>Il Cetriolo Globale</t>
+  </si>
+  <si>
+    <t>Gioschi</t>
+  </si>
+  <si>
+    <t>Peciunova</t>
+  </si>
+  <si>
+    <t>Peciu</t>
+  </si>
+  <si>
+    <t>Impepata di Cozze</t>
+  </si>
+  <si>
+    <t>Wombato</t>
+  </si>
+  <si>
+    <t>Draculino Team</t>
+  </si>
+  <si>
+    <t>Draghetto</t>
+  </si>
+  <si>
+    <t>Mandarino Bretone</t>
+  </si>
+  <si>
+    <t>Dive</t>
+  </si>
+  <si>
+    <t>Team Blizzard</t>
+  </si>
+  <si>
+    <t>Spike</t>
+  </si>
+  <si>
+    <t>S.C. Pilarella</t>
+  </si>
+  <si>
+    <t>Jocker</t>
+  </si>
+  <si>
+    <t>Personal GB</t>
+  </si>
+  <si>
+    <t>GiBi</t>
+  </si>
+  <si>
     <t>Kilkenny</t>
   </si>
   <si>
     <t>Cliath</t>
   </si>
   <si>
-    <t>Machu Picchu</t>
-  </si>
-  <si>
-    <t>Caniggia</t>
-  </si>
-  <si>
-    <t>S.C. Pilarella</t>
-  </si>
-  <si>
-    <t>Jocker</t>
-  </si>
-  <si>
-    <t>Footbears F.C.</t>
-  </si>
-  <si>
-    <t>Fatbear</t>
-  </si>
-  <si>
     <t>Corsari</t>
   </si>
   <si>
     <t>Battleaxe</t>
-  </si>
-  <si>
-    <t>Armata Brancaleone</t>
-  </si>
-  <si>
-    <t>Vervex</t>
-  </si>
-  <si>
-    <t>Pit Stop F.C.</t>
-  </si>
-  <si>
-    <t>Pit Stop</t>
-  </si>
-  <si>
-    <t>Team Blizzard</t>
-  </si>
-  <si>
-    <t>Spike</t>
-  </si>
-  <si>
-    <t>B.B. King</t>
-  </si>
-  <si>
-    <t>Remida</t>
-  </si>
-  <si>
-    <t>Ragni Domestici</t>
-  </si>
-  <si>
-    <t>Woland</t>
-  </si>
-  <si>
-    <t>Jukatan</t>
-  </si>
-  <si>
-    <t>Juk</t>
-  </si>
-  <si>
-    <t>Impepata di Cozze</t>
-  </si>
-  <si>
-    <t>Wombato</t>
-  </si>
-  <si>
-    <t>Annabella</t>
-  </si>
-  <si>
-    <t>Zag</t>
-  </si>
-  <si>
-    <t>Miami Sharks</t>
-  </si>
-  <si>
-    <t>Antoncasta</t>
-  </si>
-  <si>
-    <t>A.S. Paulina Maria</t>
-  </si>
-  <si>
-    <t>Fede235</t>
-  </si>
-  <si>
-    <t>Personal GB</t>
-  </si>
-  <si>
-    <t>GiBi</t>
-  </si>
-  <si>
-    <t>Ciak</t>
-  </si>
-  <si>
-    <t>Danbell</t>
-  </si>
-  <si>
-    <t>Jeeg Robot</t>
-  </si>
-  <si>
-    <t>Hiroshi</t>
-  </si>
-  <si>
-    <t>F.C. Ezio Glerean</t>
-  </si>
-  <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>Younes F.C.</t>
-  </si>
-  <si>
-    <t>Yeboah</t>
-  </si>
-  <si>
-    <t>Phoenix S.R.C.L.</t>
-  </si>
-  <si>
-    <t>Creator</t>
-  </si>
-  <si>
-    <t>Trimonese</t>
-  </si>
-  <si>
-    <t>Korlos</t>
-  </si>
-  <si>
-    <t>Mandarino Bretone</t>
-  </si>
-  <si>
-    <t>Dive</t>
-  </si>
-  <si>
-    <t>Cave Canem F.C.</t>
-  </si>
-  <si>
-    <t>Squaraus</t>
-  </si>
-  <si>
-    <t>Swansea F.C.</t>
-  </si>
-  <si>
-    <t>Swansea</t>
-  </si>
-  <si>
-    <t>Fantatalanta</t>
-  </si>
-  <si>
-    <t>Federico</t>
-  </si>
-  <si>
-    <t>Real Ultima</t>
-  </si>
-  <si>
-    <t>Mark Mol</t>
-  </si>
-  <si>
-    <t>Peciunova</t>
-  </si>
-  <si>
-    <t>Peciu</t>
-  </si>
-  <si>
-    <t>Il Cetriolo Globale</t>
-  </si>
-  <si>
-    <t>Gioschi</t>
-  </si>
-  <si>
-    <t>Draculino Team</t>
-  </si>
-  <si>
-    <t>Draghetto</t>
-  </si>
-  <si>
-    <t>Atletico Lupin</t>
-  </si>
-  <si>
-    <t>Santaklaus</t>
-  </si>
-  <si>
-    <t>Real Mafra</t>
-  </si>
-  <si>
-    <t>Stef</t>
   </si>
 </sst>
 </file>

</xml_diff>